<commit_message>
Updated Test Report file
</commit_message>
<xml_diff>
--- a/Test_Report.xlsx
+++ b/Test_Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manual Testing For HSC Formula Aid App\Test_Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manual Testing For HSC Formula Aid App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DB0EFA-CCC4-4507-A66E-9C4263392EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCC0C7B-759F-4E05-9389-4250DA1052E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59D7B6BC-9F3E-4222-8197-B8C49DC7222B}"/>
   </bookViews>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006458EE-7ACA-42D0-9E66-C02B47F53A96}">
   <dimension ref="A1:K2401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,14 +1626,8 @@
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I28"/>
-      <c r="K28"/>
-    </row>
-    <row r="29" spans="1:11" s="5" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I29"/>
-      <c r="K29"/>
-    </row>
+    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:11" s="5" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:11" s="5" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>

</xml_diff>